<commit_message>
convet cost driver successfully in nasa93
</commit_message>
<xml_diff>
--- a/cost_drivers.xlsx
+++ b/cost_drivers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Học tập 2025\DTU\Measurement_CMU_CS_462_NIS\AppMeasurement\App-Measurement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A23DD3A-61C0-4EF1-B0E3-8FCE74B4389B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB92EDAE-23F6-4819-8592-060CA68791B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -494,7 +494,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,11 +674,21 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="B9" s="2">
+        <v>1.46</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.71</v>
+      </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -686,19 +696,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>1.46</v>
+        <v>1.29</v>
       </c>
       <c r="C10" s="2">
-        <v>1.19</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>0.96</v>
+        <v>0.91</v>
       </c>
       <c r="F10" s="2">
-        <v>0.71</v>
+        <v>0.82</v>
       </c>
       <c r="G10" s="3"/>
     </row>
@@ -707,19 +717,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>1.29</v>
+        <v>1.42</v>
       </c>
       <c r="C11" s="2">
-        <v>1.1299999999999999</v>
+        <v>1.17</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>0.91</v>
+        <v>0.86</v>
       </c>
       <c r="F11" s="2">
-        <v>0.82</v>
+        <v>0.7</v>
       </c>
       <c r="G11" s="3"/>
     </row>
@@ -728,20 +738,18 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>1.42</v>
+        <v>1.21</v>
       </c>
       <c r="C12" s="2">
-        <v>1.17</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
       <c r="E12" s="2">
-        <v>0.86</v>
+        <v>0.9</v>
       </c>
-      <c r="F12" s="2">
-        <v>0.7</v>
-      </c>
+      <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -749,16 +757,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>1.21</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C13" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
       <c r="E13" s="2">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -768,18 +776,20 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>1.1399999999999999</v>
+        <v>1.24</v>
       </c>
       <c r="C14" s="2">
-        <v>1.07</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>0.95</v>
+        <v>0.91</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="2">
+        <v>0.82</v>
+      </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -799,7 +809,7 @@
         <v>0.91</v>
       </c>
       <c r="F15" s="2">
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -808,39 +818,29 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="C16" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="2">
-        <v>0.91</v>
+        <v>1.04</v>
       </c>
       <c r="F16" s="2">
-        <v>0.83</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="2">
-        <v>1.23</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1.08</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1.04</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -9683,12 +9683,6 @@
     </row>
     <row r="1000" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1000" s="3"/>
-      <c r="B1000" s="3"/>
-      <c r="C1000" s="3"/>
-      <c r="D1000" s="3"/>
-      <c r="E1000" s="3"/>
-      <c r="F1000" s="3"/>
-      <c r="G1000" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>